<commit_message>
Correction des filtres de carte V1
</commit_message>
<xml_diff>
--- a/Tableau_Projets.xlsx
+++ b/Tableau_Projets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lheinr02\Desktop\Cohabys\Projets\SiteWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1448" documentId="13_ncr:1_{C97D2D40-3842-4C49-98AC-CE5CAF65CF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{745D4753-5064-4005-99AD-6C087FC966C9}"/>
+  <xr:revisionPtr revIDLastSave="1545" documentId="13_ncr:1_{C97D2D40-3842-4C49-98AC-CE5CAF65CF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D44A81DE-B8DD-4673-9191-34EAC3C52018}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="396">
   <si>
     <t>🔖 Titre du projet</t>
   </si>
@@ -119,7 +119,7 @@
     <t>Biodiversité</t>
   </si>
   <si>
-    <t>Campagne en mer et suivis scientifiques</t>
+    <t>Campagnes en mer et suivis scientifiques</t>
   </si>
   <si>
     <t>Suivi DCE_Angiospermes_La Berche int HZN</t>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>https://archimer.ifremer.fr/</t>
-  </si>
-  <si>
-    <t>Campagne intertidal et suivis scientifiques</t>
   </si>
   <si>
     <t>Suivi DCE_MIB_Boyardville SM</t>
@@ -283,9 +280,6 @@
     <t>Dans le cadre du projet RECIF 17 visant à l’implantation de récifs artificiels au large de l’île d’Oléron, 6 années de suivis post-immersion de la faune fixée ont été réalisés. Ce suivi a pour but d’évaluer la colonisation des structures par la faune fixée au cours d’un suivi dans le temps.</t>
   </si>
   <si>
-    <t>Suivis scientifiques</t>
-  </si>
-  <si>
     <t>Étude biosédimentaire du « Port de Rivedoux-Plage »</t>
   </si>
   <si>
@@ -316,7 +310,7 @@
     <t>,</t>
   </si>
   <si>
-    <t>Campagne géophysique</t>
+    <t>Campagnes géophysiques</t>
   </si>
   <si>
     <t>Campagne GARANTI</t>
@@ -346,7 +340,7 @@
     <t>Energies Marines Renouvelables</t>
   </si>
   <si>
-    <t>Analyse de données</t>
+    <t>Analyses de données</t>
   </si>
   <si>
     <t>RESPECT</t>
@@ -427,9 +421,6 @@
     <t>46,848443 ; -2,392589</t>
   </si>
   <si>
-    <t>Analyses de données</t>
-  </si>
-  <si>
     <t>Etude d'impact EMDT</t>
   </si>
   <si>
@@ -511,7 +502,7 @@
     <t>49,831222 ; 0,218456</t>
   </si>
   <si>
-    <t>Conseil, expertise</t>
+    <t>Conseil et expertise</t>
   </si>
   <si>
     <t>AO1 Courseulles</t>
@@ -637,7 +628,7 @@
     <t>https://lnkd.in/ehjfRGpK</t>
   </si>
   <si>
-    <t>Conseil, expertise ; Analyse de données</t>
+    <t>Conseil et expertise ; Analyses de données</t>
   </si>
   <si>
     <t>AMO DGEC Façade NAMO</t>
@@ -661,7 +652,7 @@
     <t>42,906152 ; 4,054442</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://lnkd.in/ev54SRuf </t>
+    <t xml:space="preserve">https://lnkd.in/ev54SRuf </t>
   </si>
   <si>
     <t>AMO DGEC AO4</t>
@@ -676,9 +667,6 @@
     <t>49,607420 ; -0.606302</t>
   </si>
   <si>
-    <t>conseil, expertise</t>
-  </si>
-  <si>
     <t>AMO DGEC AO5</t>
   </si>
   <si>
@@ -742,7 +730,7 @@
     <t>47,577002 ; -3 ,965539</t>
   </si>
   <si>
-    <t>Campagnes en mer ; analyse de données</t>
+    <t>Campagnes en mer et suivis scientifiques ; Analyses de données</t>
   </si>
   <si>
     <t>EOLE</t>
@@ -772,7 +760,7 @@
     <t>Exploitation ressources minières</t>
   </si>
   <si>
-    <t>Analyse de données ; campagne en mer et suivis scientifiques</t>
+    <t>Analyses de données ; Campagnes en mer et suivis scientifiques</t>
   </si>
   <si>
     <t>Formation PALR</t>
@@ -1009,7 +997,7 @@
     <t>42,698034 ; 9 ,454543</t>
   </si>
   <si>
-    <t>Conseil, expertise ; formation</t>
+    <t>Conseil et expertise ; Formation</t>
   </si>
   <si>
     <t>Surveillance visuelle de la mégafaune marine dans le cadre du chantier d’atterrage du câble du parc éolien de St Brieuc (Nexans).  Mise à disposition d’observateurs à terre pour surveillance régulière du chantier et mise en place de mesures de mitigation (un jour par semaine pendant 4 mois). </t>
@@ -1069,6 +1057,9 @@
     <t>46,688810 ; -3,855811</t>
   </si>
   <si>
+    <t>Campagne en mer et suivis scientifiques</t>
+  </si>
+  <si>
     <t>Platin de Grave</t>
   </si>
   <si>
@@ -1117,9 +1108,6 @@
     <t>1,912104 ; -79 ,249334</t>
   </si>
   <si>
-    <t>Campagnes en mer et suivis scientifiques</t>
-  </si>
-  <si>
     <t xml:space="preserve">Etat de référence FEC </t>
   </si>
   <si>
@@ -1165,7 +1153,7 @@
     <t>48,800799 ; 2.341647</t>
   </si>
   <si>
-    <t>Biodiversité ; exploitation de ressources minières</t>
+    <t>Biodiversité ; Exploitation ressources minières</t>
   </si>
   <si>
     <t>Campagne Guyane</t>
@@ -1178,9 +1166,6 @@
   </si>
   <si>
     <t>6,011921 ; -51,913903</t>
-  </si>
-  <si>
-    <t>Campagnes en mer et suivis scientifiques ; Analyses de données</t>
   </si>
   <si>
     <t>EBS Liban</t>
@@ -1223,9 +1208,6 @@
 - https://lnkd.in/gvfTrjTy</t>
   </si>
   <si>
-    <t>Analyse de données ; campagnes en mer et suivis scientifiques</t>
-  </si>
-  <si>
     <t>Campagne SEFASIL</t>
   </si>
   <si>
@@ -1247,14 +1229,14 @@
     <t>Participation à l’état initial de la mégafaune marine dans le cadre d’un projet de forage en Guyane. Mise à disposition de 3 observateurs de faune marine pendant un mois, analyse des données visuelles et acoustiques, rapport final. </t>
   </si>
   <si>
-    <t>-https://lnkd.in/gqik27Vn</t>
+    <t>https://lnkd.in/gqik27Vn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1341,12 +1323,6 @@
       <sz val="12"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF242424"/>
-      <name val="Consolas"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1486,7 +1462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1494,31 +1470,30 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2067,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="F54" workbookViewId="0">
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2086,60 +2061,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:10" hidden="1">
       <c r="A4" t="s">
@@ -2189,7 +2164,7 @@
       <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="25" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -2217,7 +2192,7 @@
       <c r="E6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -2230,28 +2205,28 @@
         <v>25</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>32</v>
@@ -2265,23 +2240,23 @@
     </row>
     <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>36</v>
+      <c r="F8" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>32</v>
@@ -2290,28 +2265,28 @@
         <v>25</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>36</v>
+      <c r="F9" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>32</v>
@@ -2320,28 +2295,28 @@
         <v>25</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>32</v>
@@ -2350,28 +2325,28 @@
         <v>25</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75">
       <c r="A11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>36</v>
+      <c r="F11" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>32</v>
@@ -2385,23 +2360,23 @@
     </row>
     <row r="12" spans="1:10" ht="15.75">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>44</v>
+      <c r="F12" s="25" t="s">
+        <v>43</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>32</v>
@@ -2415,23 +2390,23 @@
     </row>
     <row r="13" spans="1:10" ht="15.75">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>32</v>
@@ -2445,7 +2420,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>28</v>
@@ -2457,11 +2432,11 @@
       <c r="E14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>32</v>
@@ -2470,12 +2445,12 @@
         <v>25</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>28</v>
@@ -2487,11 +2462,11 @@
       <c r="E15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>32</v>
@@ -2500,28 +2475,28 @@
         <v>25</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
       <c r="A16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>32</v>
@@ -2530,28 +2505,28 @@
         <v>25</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>58</v>
+      <c r="F17" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>32</v>
@@ -2560,28 +2535,28 @@
         <v>25</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75">
       <c r="A18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="27" t="s">
-        <v>58</v>
+      <c r="F18" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>32</v>
@@ -2590,12 +2565,12 @@
         <v>25</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75">
       <c r="A19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>28</v>
@@ -2607,11 +2582,11 @@
       <c r="E19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>32</v>
@@ -2625,23 +2600,23 @@
     </row>
     <row r="20" spans="1:10" ht="15.75">
       <c r="A20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>32</v>
@@ -2650,61 +2625,61 @@
         <v>25</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75">
       <c r="A21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="6">
         <v>2021</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="H21" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="27" t="s">
-        <v>58</v>
+      <c r="F22" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="G22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>25</v>
@@ -2715,87 +2690,87 @@
     </row>
     <row r="23" spans="1:10" ht="15.75">
       <c r="A23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="C23" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>79</v>
+      <c r="F23" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="G23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75">
       <c r="A24" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" s="6">
         <v>2021</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="27" t="s">
-        <v>83</v>
+      <c r="F24" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75">
       <c r="A25" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B25" s="6">
         <v>2017</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="H25" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="I25" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>26</v>
@@ -2803,27 +2778,27 @@
     </row>
     <row r="26" spans="1:10" ht="15.75">
       <c r="A26" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="6">
         <v>2017</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>26</v>
@@ -2831,89 +2806,89 @@
     </row>
     <row r="27" spans="1:10" ht="15.75">
       <c r="A27" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B27" s="6">
         <v>2017</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="G27" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>99</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75">
       <c r="A28" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="D28" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="G28" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="H28" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="I28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75">
       <c r="A29" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" s="6">
         <v>2016</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>26</v>
@@ -2921,27 +2896,27 @@
     </row>
     <row r="30" spans="1:10" ht="15.75">
       <c r="A30" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" s="6">
         <v>2016</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>26</v>
@@ -2949,27 +2924,27 @@
     </row>
     <row r="31" spans="1:10" ht="15.75">
       <c r="A31" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="6">
         <v>2016</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>26</v>
@@ -2977,27 +2952,27 @@
     </row>
     <row r="32" spans="1:10" ht="15.75">
       <c r="A32" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B32" s="6">
         <v>2016</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>26</v>
@@ -3005,87 +2980,87 @@
     </row>
     <row r="33" spans="1:10" ht="15.75">
       <c r="A33" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B33" s="6">
         <v>2016</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="G33" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75">
       <c r="A34" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B34" s="6">
         <v>2016</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.75">
       <c r="A35" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B35" s="6">
         <v>2015</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>26</v>
@@ -3093,57 +3068,57 @@
     </row>
     <row r="36" spans="1:10" ht="15.75">
       <c r="A36" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B36" s="6">
         <v>2015</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75">
       <c r="A37" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B37" s="6">
         <v>2014</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>26</v>
@@ -3151,253 +3126,253 @@
     </row>
     <row r="38" spans="1:10" ht="15.75">
       <c r="A38" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B38" s="6">
         <v>2014</v>
       </c>
       <c r="C38" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>146</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75">
       <c r="A39" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B39" s="6">
         <v>2014</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75">
       <c r="A40" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B40" s="6">
         <v>2013</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75">
       <c r="A41" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B41" s="6">
         <v>2013</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75">
       <c r="A42" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B42" s="6">
         <v>2013</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75">
       <c r="A43" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B43" s="6">
         <v>2013</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75">
       <c r="A44" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B44" s="6">
         <v>2012</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75">
       <c r="A45" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B45" s="6">
         <v>2012</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15.75">
       <c r="A46" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B46" s="6">
         <v>2011</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>26</v>
@@ -3405,513 +3380,513 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B47" s="6">
         <v>2011</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="G48" s="17" t="s">
         <v>182</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>185</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="E49" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="G49" s="17" t="s">
         <v>188</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="G50" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="H50" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F50" s="18" t="s">
+      <c r="I50" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J50" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="H50" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F51" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J51" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F52" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J52" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="H52" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J52" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="5" customFormat="1">
       <c r="A53" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F53" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J53" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="H53" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J53" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="G54" s="17" t="s">
         <v>207</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>210</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F55" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="G55" s="17" t="s">
         <v>209</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>213</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>217</v>
+        <v>212</v>
+      </c>
+      <c r="H56" s="19" t="s">
+        <v>213</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="H57" s="22" t="s">
-        <v>221</v>
+        <v>216</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>217</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F58" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="G58" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="H58" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>228</v>
-      </c>
       <c r="I58" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G59" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B60" s="6">
         <v>2025</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B61" s="6">
         <v>2025</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F61" s="23" t="s">
-        <v>240</v>
+        <v>85</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>236</v>
       </c>
       <c r="G61" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B62" s="6">
         <v>2025</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B63" s="6">
         <v>2025</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>251</v>
+        <v>85</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J63" s="6" t="s">
         <v>26</v>
@@ -3919,55 +3894,55 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B64" s="6">
         <v>2025</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>254</v>
+        <v>85</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>250</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B65" s="6">
         <v>2024</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J65" s="6" t="s">
         <v>26</v>
@@ -3976,27 +3951,27 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B66" s="6">
         <v>2024</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G66" s="17" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>26</v>
@@ -4004,173 +3979,173 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B67" s="6">
         <v>2024</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F67" s="24" t="s">
-        <v>263</v>
+        <v>104</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>259</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B68" s="6">
         <v>2024</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G68" s="17" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B69" s="6">
         <v>2024</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F69" s="23" t="s">
-        <v>270</v>
+        <v>85</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>266</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B70" s="6">
         <v>2023</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F70" s="23" t="s">
-        <v>273</v>
+        <v>85</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>269</v>
       </c>
       <c r="G70" s="17" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B71" s="6">
         <v>2023</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F71" s="23" t="s">
-        <v>276</v>
+        <v>85</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>272</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B72" s="6">
         <v>2023</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>26</v>
@@ -4178,113 +4153,113 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B73" s="6">
         <v>2023</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G73" s="17" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B74" s="6">
         <v>2023</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B75" s="6">
         <v>2023</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B76" s="6">
         <v>2022</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>26</v>
@@ -4292,27 +4267,27 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B77" s="6">
         <v>2022</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>26</v>
@@ -4320,23 +4295,23 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B78" s="6">
         <v>2022</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H78" s="6"/>
       <c r="I78" s="6" t="s">
@@ -4348,23 +4323,23 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B79" s="6">
         <v>2022</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="6" t="s">
@@ -4376,27 +4351,27 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B80" s="6">
         <v>2022</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F80" s="18" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J80" s="6" t="s">
         <v>26</v>
@@ -4404,27 +4379,27 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B81" s="6">
         <v>2022</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F81" s="18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J81" s="6" t="s">
         <v>26</v>
@@ -4432,115 +4407,115 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="6" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B82" s="6">
         <v>2022</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F82" s="18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B83" s="6">
         <v>2022</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G83" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B84" s="6">
         <v>2022</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F84" s="18" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H84" s="6"/>
       <c r="I84" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B85" s="6">
         <v>2022</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F85" s="18" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G85" s="17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H85" s="6"/>
       <c r="I85" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J85" s="6" t="s">
         <v>26</v>
@@ -4548,85 +4523,85 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B86" s="6">
         <v>2021</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F86" s="18" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H86" s="6"/>
       <c r="I86" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B87" s="6">
         <v>2021</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F87" s="18" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H87" s="6"/>
       <c r="I87" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J87" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B88" s="6">
         <v>2021</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F88" s="23" t="s">
-        <v>330</v>
+        <v>85</v>
+      </c>
+      <c r="F88" s="21" t="s">
+        <v>326</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H88" s="6"/>
       <c r="I88" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J88" s="6" t="s">
         <v>26</v>
@@ -4634,27 +4609,27 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B89" s="6">
         <v>2021</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F89" s="18" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G89" s="17" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H89" s="6"/>
       <c r="I89" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J89" s="6" t="s">
         <v>26</v>
@@ -4662,383 +4637,383 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B90" s="6">
         <v>2021</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F90" s="18" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G90" s="17" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H90" s="6"/>
       <c r="I90" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="6" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B91" s="6">
         <v>2021</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G91" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H91" s="6"/>
       <c r="I91" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>26</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="6" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B92" s="6">
         <v>2021</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G92" s="17" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H92" s="6"/>
       <c r="I92" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B93" s="6">
         <v>2021</v>
       </c>
       <c r="C93" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F93" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="G93" s="17" t="s">
         <v>347</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F93" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>350</v>
       </c>
       <c r="H93" s="6"/>
       <c r="I93" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="6" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B94" s="6">
         <v>2021</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G94" s="17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H94" s="6"/>
       <c r="I94" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J94" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="6" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B95" s="6">
         <v>2020</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F95" s="18" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G95" s="17" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="H95" s="6"/>
       <c r="I95" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J95" s="6" t="s">
-        <v>358</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B96" s="6">
         <v>2020</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F96" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G96" s="25" t="s">
-        <v>361</v>
+        <v>356</v>
+      </c>
+      <c r="G96" s="23" t="s">
+        <v>357</v>
       </c>
       <c r="H96" s="6"/>
       <c r="I96" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J96" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B97" s="6">
         <v>2020</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F97" s="18" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G97" s="17" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H97" s="6"/>
       <c r="I97" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B98" s="6">
         <v>2020</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F98" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="G98" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="H98" s="13" t="s">
         <v>366</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F98" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="G98" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>370</v>
       </c>
       <c r="I98" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J98" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B99" s="6">
         <v>2020</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D99" s="6"/>
       <c r="E99" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F99" s="18" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G99" s="17" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H99" s="6"/>
       <c r="I99" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J99" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B100" s="6">
         <v>2019</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F100" s="23" t="s">
-        <v>377</v>
+        <v>85</v>
+      </c>
+      <c r="F100" s="21" t="s">
+        <v>373</v>
       </c>
       <c r="G100" s="17" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H100" s="6"/>
       <c r="I100" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J100" s="6" t="s">
-        <v>379</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="6" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B101" s="6">
         <v>2019</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F101" s="23" t="s">
-        <v>381</v>
+        <v>85</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>376</v>
       </c>
       <c r="G101" s="17" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="H101" s="6"/>
       <c r="I101" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J101" s="6" t="s">
-        <v>379</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B102" s="6">
         <v>2019</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F102" s="18" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G102" s="17" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="H102" s="6"/>
       <c r="I102" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J102" s="6" t="s">
         <v>26</v>
@@ -5046,186 +5021,174 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="6" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B103" s="6">
         <v>2019</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F103" s="23" t="s">
-        <v>388</v>
+        <v>85</v>
+      </c>
+      <c r="F103" s="21" t="s">
+        <v>383</v>
       </c>
       <c r="G103" s="17" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H103" s="6"/>
       <c r="I103" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B104" s="6">
         <v>2018</v>
       </c>
       <c r="C104" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="G104" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="H104" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="J104" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F104" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="G104" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="I104" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="J104" s="6" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="6" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B105" s="6">
         <v>2018</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F105" s="18" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="H105" s="26"/>
+        <v>390</v>
+      </c>
+      <c r="H105" s="24"/>
       <c r="I105" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J105" s="6" t="s">
-        <v>358</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="6" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B106" s="6">
         <v>2018</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="G106" s="17" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="H106" s="6"/>
       <c r="I106" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J106" s="6" t="s">
-        <v>358</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B107" s="6">
         <v>2017</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F107" s="18" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G107" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="H107" s="6" t="s">
-        <v>401</v>
+        <v>386</v>
+      </c>
+      <c r="H107" s="19" t="s">
+        <v>395</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J107" s="6" t="s">
-        <v>379</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J6">
-      <sortCondition ref="A1:A3"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J3">
+      <sortCondition ref="I1:I3"/>
     </sortState>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="I27:I28 I33:I34 I36 I38:I45 I47:I79 I82:I107 I4:I24">
+  <conditionalFormatting sqref="I27:I28 I33:I34 I36 I38:I45 I47:I64 I82:I87 I4:I24 I67:I68 I70:I75 I77:I79 I90:I94 I96:I107">
     <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J32">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5248,7 +5211,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33:J107 K65 J4:J28">
+  <conditionalFormatting sqref="J4:J107 K65">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -5279,25 +5242,21 @@
     <hyperlink ref="H8:H13" r:id="rId16" xr:uid="{B3BAADF8-8196-429E-8B14-D6B7446814E1}"/>
     <hyperlink ref="H56" r:id="rId17" xr:uid="{E314C7C6-78E4-4D38-ABBD-DC20D64FFC6A}"/>
     <hyperlink ref="H21" r:id="rId18" xr:uid="{D07B2664-3265-4714-B738-9294A4BADDA2}"/>
+    <hyperlink ref="H107" r:id="rId19" xr:uid="{2DEEB027-FF12-496A-8730-C7F207D08F47}"/>
+    <hyperlink ref="H51" r:id="rId20" xr:uid="{4AB30B8A-26D6-46FB-BF61-8E291B2BF7F8}"/>
+    <hyperlink ref="H53" r:id="rId21" xr:uid="{F0E1E216-2153-4AE1-A2C9-5C167B489CE6}"/>
+    <hyperlink ref="H52" r:id="rId22" xr:uid="{C389B2A7-727C-415A-8CF8-50F793143B6F}"/>
+    <hyperlink ref="H50" r:id="rId23" xr:uid="{8E782F87-15E7-4DB4-BFD6-9DF4B4870889}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABE9AB3B7329F749871879A420148C1E" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="98c86cbeda78977a99426c9df0db3802">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4a73538-f369-420a-9543-938e8918f479" xmlns:ns3="6cc7a583-fbb3-442c-ac3d-339523f19a40" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d3f6fe07b66778c70bfdc858ced9d8b6" ns2:_="" ns3:_="">
     <xsd:import namespace="c4a73538-f369-420a-9543-938e8918f479"/>
@@ -5498,6 +5457,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5510,11 +5478,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F8297D-C590-4260-B1A7-42866958BEC5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BE83C2B-BBFC-4DF8-BD2C-DEC7C4F3E0ED}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BE83C2B-BBFC-4DF8-BD2C-DEC7C4F3E0ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F8297D-C590-4260-B1A7-42866958BEC5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Correction des filtres de cartes V3
</commit_message>
<xml_diff>
--- a/Tableau_Projets.xlsx
+++ b/Tableau_Projets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lheinr02\Desktop\Cohabys\Projets\SiteWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1545" documentId="13_ncr:1_{C97D2D40-3842-4C49-98AC-CE5CAF65CF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D44A81DE-B8DD-4673-9191-34EAC3C52018}"/>
+  <xr:revisionPtr revIDLastSave="1550" documentId="13_ncr:1_{C97D2D40-3842-4C49-98AC-CE5CAF65CF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{660F7250-3426-4228-B7B3-FAB584E6AF9C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="395">
   <si>
     <t>🔖 Titre du projet</t>
   </si>
@@ -265,7 +265,7 @@
     <t>CAPENA</t>
   </si>
   <si>
-    <t>46,1 ; -1,33</t>
+    <t>46,02 ; -1,56</t>
   </si>
   <si>
     <t>http://recif17.blogspot.com/; https://www.cape-na.fr/wp-content/uploads/2024/06/Bilan_finalRECIF17.pdf</t>
@@ -1055,9 +1055,6 @@
   </si>
   <si>
     <t>46,688810 ; -3,855811</t>
-  </si>
-  <si>
-    <t>Campagne en mer et suivis scientifiques</t>
   </si>
   <si>
     <t>Platin de Grave</t>
@@ -1740,7 +1737,16 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C6DD9AFC-E311-4B3B-873C-4F9832BE501C}" name="Table2" displayName="Table2" ref="A4:H107" totalsRowShown="0" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="A4:H107" xr:uid="{C6DD9AFC-E311-4B3B-873C-4F9832BE501C}"/>
+  <autoFilter ref="A4:H107" xr:uid="{C6DD9AFC-E311-4B3B-873C-4F9832BE501C}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E98917CF-698A-43D8-80F2-F95853FC538C}" name="Column1" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{8DC19361-6619-44CD-ADF8-C7F25031D5C9}" name="Column2" dataDxfId="6"/>
@@ -2040,10 +2046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F54" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2092,7 +2099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1">
+    <row r="2" spans="1:10" ht="15" hidden="1" customHeight="1">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -2104,7 +2111,7 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1">
+    <row r="3" spans="1:10" ht="15" hidden="1" customHeight="1">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -4690,18 +4697,18 @@
         <v>25</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>338</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B92" s="6">
         <v>2021</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>95</v>
@@ -4710,10 +4717,10 @@
         <v>85</v>
       </c>
       <c r="F92" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="G92" s="17" t="s">
         <v>341</v>
-      </c>
-      <c r="G92" s="17" t="s">
-        <v>342</v>
       </c>
       <c r="H92" s="6"/>
       <c r="I92" s="6" t="s">
@@ -4725,25 +4732,25 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B93" s="6">
         <v>2021</v>
       </c>
       <c r="C93" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="E93" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F93" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="E93" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F93" s="18" t="s">
+      <c r="G93" s="17" t="s">
         <v>346</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>347</v>
       </c>
       <c r="H93" s="6"/>
       <c r="I93" s="6" t="s">
@@ -4755,23 +4762,23 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B94" s="6">
         <v>2021</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F94" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="G94" s="17" t="s">
         <v>350</v>
-      </c>
-      <c r="G94" s="17" t="s">
-        <v>351</v>
       </c>
       <c r="H94" s="6"/>
       <c r="I94" s="6" t="s">
@@ -4783,7 +4790,7 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B95" s="6">
         <v>2020</v>
@@ -4796,10 +4803,10 @@
         <v>85</v>
       </c>
       <c r="F95" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="G95" s="17" t="s">
         <v>353</v>
-      </c>
-      <c r="G95" s="17" t="s">
-        <v>354</v>
       </c>
       <c r="H95" s="6"/>
       <c r="I95" s="6" t="s">
@@ -4811,7 +4818,7 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B96" s="6">
         <v>2020</v>
@@ -4826,10 +4833,10 @@
         <v>85</v>
       </c>
       <c r="F96" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="G96" s="23" t="s">
         <v>356</v>
-      </c>
-      <c r="G96" s="23" t="s">
-        <v>357</v>
       </c>
       <c r="H96" s="6"/>
       <c r="I96" s="6" t="s">
@@ -4841,7 +4848,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B97" s="6">
         <v>2020</v>
@@ -4856,10 +4863,10 @@
         <v>85</v>
       </c>
       <c r="F97" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="G97" s="17" t="s">
         <v>359</v>
-      </c>
-      <c r="G97" s="17" t="s">
-        <v>360</v>
       </c>
       <c r="H97" s="6"/>
       <c r="I97" s="6" t="s">
@@ -4871,28 +4878,28 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B98" s="6">
         <v>2020</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="E98" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F98" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="E98" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F98" s="18" t="s">
+      <c r="G98" s="17" t="s">
         <v>364</v>
       </c>
-      <c r="G98" s="17" t="s">
+      <c r="H98" s="13" t="s">
         <v>365</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>366</v>
       </c>
       <c r="I98" s="6" t="s">
         <v>25</v>
@@ -4903,7 +4910,7 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B99" s="6">
         <v>2020</v>
@@ -4916,14 +4923,14 @@
         <v>85</v>
       </c>
       <c r="F99" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="G99" s="17" t="s">
         <v>368</v>
-      </c>
-      <c r="G99" s="17" t="s">
-        <v>369</v>
       </c>
       <c r="H99" s="6"/>
       <c r="I99" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J99" s="6" t="s">
         <v>195</v>
@@ -4931,7 +4938,7 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B100" s="6">
         <v>2019</v>
@@ -4940,16 +4947,16 @@
         <v>235</v>
       </c>
       <c r="D100" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F100" s="21" t="s">
         <v>372</v>
       </c>
-      <c r="E100" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F100" s="21" t="s">
+      <c r="G100" s="17" t="s">
         <v>373</v>
-      </c>
-      <c r="G100" s="17" t="s">
-        <v>374</v>
       </c>
       <c r="H100" s="6"/>
       <c r="I100" s="6" t="s">
@@ -4961,7 +4968,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B101" s="6">
         <v>2019</v>
@@ -4976,10 +4983,10 @@
         <v>85</v>
       </c>
       <c r="F101" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="G101" s="17" t="s">
         <v>376</v>
-      </c>
-      <c r="G101" s="17" t="s">
-        <v>377</v>
       </c>
       <c r="H101" s="6"/>
       <c r="I101" s="6" t="s">
@@ -4991,13 +4998,13 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B102" s="6">
         <v>2019</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>95</v>
@@ -5006,10 +5013,10 @@
         <v>85</v>
       </c>
       <c r="F102" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="G102" s="17" t="s">
         <v>379</v>
-      </c>
-      <c r="G102" s="17" t="s">
-        <v>380</v>
       </c>
       <c r="H102" s="6"/>
       <c r="I102" s="6" t="s">
@@ -5021,25 +5028,25 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B103" s="6">
         <v>2019</v>
       </c>
       <c r="C103" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F103" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="D103" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F103" s="21" t="s">
+      <c r="G103" s="17" t="s">
         <v>383</v>
-      </c>
-      <c r="G103" s="17" t="s">
-        <v>384</v>
       </c>
       <c r="H103" s="6"/>
       <c r="I103" s="6" t="s">
@@ -5051,7 +5058,7 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B104" s="6">
         <v>2018</v>
@@ -5066,13 +5073,13 @@
         <v>85</v>
       </c>
       <c r="F104" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="G104" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="G104" s="17" t="s">
+      <c r="H104" s="13" t="s">
         <v>386</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>387</v>
       </c>
       <c r="I104" s="6" t="s">
         <v>238</v>
@@ -5083,7 +5090,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B105" s="6">
         <v>2018</v>
@@ -5096,10 +5103,10 @@
         <v>85</v>
       </c>
       <c r="F105" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="G105" s="10" t="s">
         <v>389</v>
-      </c>
-      <c r="G105" s="10" t="s">
-        <v>390</v>
       </c>
       <c r="H105" s="24"/>
       <c r="I105" s="6" t="s">
@@ -5111,7 +5118,7 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B106" s="6">
         <v>2018</v>
@@ -5124,10 +5131,10 @@
         <v>85</v>
       </c>
       <c r="F106" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="G106" s="17" t="s">
         <v>392</v>
-      </c>
-      <c r="G106" s="17" t="s">
-        <v>393</v>
       </c>
       <c r="H106" s="6"/>
       <c r="I106" s="6" t="s">
@@ -5139,7 +5146,7 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B107" s="6">
         <v>2017</v>
@@ -5154,13 +5161,13 @@
         <v>85</v>
       </c>
       <c r="F107" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="G107" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="H107" s="19" t="s">
         <v>394</v>
-      </c>
-      <c r="G107" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="H107" s="19" t="s">
-        <v>395</v>
       </c>
       <c r="I107" s="6" t="s">
         <v>238</v>
@@ -5171,7 +5178,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J3">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="capena"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J5">
       <sortCondition ref="I1:I3"/>
     </sortState>
   </autoFilter>
@@ -5257,6 +5269,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4a73538-f369-420a-9543-938e8918f479">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6cc7a583-fbb3-442c-ac3d-339523f19a40" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABE9AB3B7329F749871879A420148C1E" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="98c86cbeda78977a99426c9df0db3802">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4a73538-f369-420a-9543-938e8918f479" xmlns:ns3="6cc7a583-fbb3-442c-ac3d-339523f19a40" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d3f6fe07b66778c70bfdc858ced9d8b6" ns2:_="" ns3:_="">
     <xsd:import namespace="c4a73538-f369-420a-9543-938e8918f479"/>
@@ -5457,7 +5480,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5466,25 +5489,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4a73538-f369-420a-9543-938e8918f479">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6cc7a583-fbb3-442c-ac3d-339523f19a40" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55976C62-4295-4E18-8720-90D69C108101}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BE83C2B-BBFC-4DF8-BD2C-DEC7C4F3E0ED}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F8297D-C590-4260-B1A7-42866958BEC5}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55976C62-4295-4E18-8720-90D69C108101}"/>
 </file>
</xml_diff>